<commit_message>
worked data downloader with the team and had George help. Starting if/else
</commit_message>
<xml_diff>
--- a/sql/library-abq-all.xlsx
+++ b/sql/library-abq-all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slimg\Desktop\bootcamp\Git\little-library\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812C7E62-D05D-4732-85D8-C44CB0AA9E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC5ECF8-EEEA-40F6-AFC5-35D666DD7ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="4635" windowWidth="22800" windowHeight="16305" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
+    <workbookView xWindow="-26310" yWindow="9510" windowWidth="21960" windowHeight="12330" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,9 +377,6 @@
     <t>library_lat</t>
   </si>
   <si>
-    <t>library_eventOptIn</t>
-  </si>
-  <si>
     <t>library_description</t>
   </si>
   <si>
@@ -567,6 +564,9 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>library_event_opt_in</t>
   </si>
 </sst>
 </file>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF696C8F-C0BA-4CFB-9733-D4AF25C2BA9E}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -974,19 +974,19 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>111</v>
@@ -1024,7 +1024,7 @@
         <v>104</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>0</v>
@@ -1076,7 +1076,7 @@
         <v>97</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>0</v>
@@ -1154,7 +1154,7 @@
         <v>87</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>0</v>
@@ -1217,7 +1217,7 @@
         <v>79</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E10" s="1" t="b">
         <v>1</v>
@@ -1232,7 +1232,7 @@
         <v>78</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>0</v>
@@ -1269,7 +1269,7 @@
         <v>73</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E12" s="1" t="b">
         <v>1</v>
@@ -1295,7 +1295,7 @@
         <v>70</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E13" s="1" t="b">
         <v>0</v>
@@ -1310,7 +1310,7 @@
         <v>69</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>0</v>
@@ -1347,7 +1347,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E15" s="1" t="b">
         <v>0</v>
@@ -1425,7 +1425,7 @@
         <v>53</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E18" s="1" t="b">
         <v>1</v>
@@ -1440,7 +1440,7 @@
         <v>52</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>0</v>
@@ -1596,7 +1596,7 @@
         <v>31</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>0</v>
@@ -1778,7 +1778,7 @@
         <v>7</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>0</v>
@@ -1789,7 +1789,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E32" s="1" t="b">
         <v>1</v>
@@ -1804,7 +1804,7 @@
         <v>5</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>0</v>
@@ -1838,10 +1838,10 @@
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C34" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E34" s="1" t="b">
         <v>0</v>
@@ -1853,21 +1853,21 @@
         <v>-106.70972</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C35" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E35" s="1" t="b">
         <v>0</v>
@@ -1879,21 +1879,21 @@
         <v>-106.72486000000001</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C36" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E36" s="1" t="b">
         <v>0</v>
@@ -1905,21 +1905,21 @@
         <v>-106.5558</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C37" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E37" s="1" t="b">
         <v>0</v>
@@ -1931,21 +1931,21 @@
         <v>-106.38930000000001</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C38" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E38" s="1" t="b">
         <v>0</v>
@@ -1957,21 +1957,21 @@
         <v>-106.58564</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C39" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E39" s="1" t="b">
         <v>0</v>
@@ -1983,21 +1983,21 @@
         <v>-106.61281</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C40" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E40" s="1" t="b">
         <v>0</v>
@@ -2009,21 +2009,21 @@
         <v>-106.56204</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C41" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E41" s="1" t="b">
         <v>0</v>
@@ -2035,21 +2035,21 @@
         <v>-106.51611</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C42" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E42" s="1" t="b">
         <v>0</v>
@@ -2061,21 +2061,21 @@
         <v>-106.49758</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C43" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E43" s="1" t="b">
         <v>0</v>
@@ -2087,21 +2087,21 @@
         <v>-106.64831</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C44" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E44" s="1" t="b">
         <v>0</v>
@@ -2113,21 +2113,21 @@
         <v>-106.65331999999999</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C45" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E45" s="1" t="b">
         <v>0</v>
@@ -2139,21 +2139,21 @@
         <v>-106.62716</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C46" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E46" s="1" t="b">
         <v>0</v>
@@ -2165,21 +2165,21 @@
         <v>-106.57723</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C47" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E47" s="1" t="b">
         <v>0</v>
@@ -2191,21 +2191,21 @@
         <v>-106.64546</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C48" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E48" s="1" t="b">
         <v>0</v>
@@ -2217,21 +2217,21 @@
         <v>-106.68216</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C49" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E49" s="1" t="b">
         <v>0</v>
@@ -2243,21 +2243,21 @@
         <v>-106.64216999999999</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C50" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E50" s="1" t="b">
         <v>0</v>
@@ -2269,21 +2269,21 @@
         <v>-106.71614</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C51" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E51" s="1" t="b">
         <v>0</v>
@@ -2295,21 +2295,21 @@
         <v>-106.55294000000001</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C52" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E52" s="1" t="b">
         <v>0</v>
@@ -2321,13 +2321,13 @@
         <v>-106.75161</v>
       </c>
       <c r="H52" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J52" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data downloded file updates, pins reset back to LL and PL
</commit_message>
<xml_diff>
--- a/sql/library-abq-all.xlsx
+++ b/sql/library-abq-all.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slimg\Desktop\bootcamp\Git\little-library\sql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nycoledavila/Desktop/DDC WEB /Git/little-library/sql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA7529F3-FE27-4227-92F2-4C5AC9B4AD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E411F3-5B0F-3E43-8D09-A842CCC270FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21075" yWindow="12180" windowWidth="19725" windowHeight="10875" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
+    <workbookView xWindow="80" yWindow="800" windowWidth="35840" windowHeight="19500" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="165">
   <si>
     <t>Little Library</t>
   </si>
   <si>
-    <t>children</t>
-  </si>
-  <si>
     <t>La Luz</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>6467 Brenton Dr Nw, Albuquerque, NM 87120</t>
   </si>
   <si>
-    <t>romance</t>
-  </si>
-  <si>
     <t>Cheryl Olsen #89915 </t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>6219 Cochiti Dr NW, Albuquerque, NM 87120</t>
   </si>
   <si>
-    <t>home improvement</t>
-  </si>
-  <si>
     <t>The Road to Santiago</t>
   </si>
   <si>
@@ -108,9 +99,6 @@
   </si>
   <si>
     <t>3800 Torrey Pines RD Se, Rio Rancho,NM,87124</t>
-  </si>
-  <si>
-    <t>fiction</t>
   </si>
   <si>
     <t>Regina Padilla #20175 </t>
@@ -161,9 +149,6 @@
     <t>4208 Stowe Rd Nw, Albuquerque, NM 87114</t>
   </si>
   <si>
-    <t>car</t>
-  </si>
-  <si>
     <t>Condessa library</t>
   </si>
   <si>
@@ -182,9 +167,6 @@
     <t>4420 Condesa Ct Nw, Albuquerque, NM 87114</t>
   </si>
   <si>
-    <t>Fantasy</t>
-  </si>
-  <si>
     <t>Jennifer Lucero</t>
   </si>
   <si>
@@ -203,9 +185,6 @@
     <t>411 Aliso Dr. Se, Albuquerque, NM</t>
   </si>
   <si>
-    <t>Satire</t>
-  </si>
-  <si>
     <t>Carolyn and Ken's Library &amp; Micro Pantry</t>
   </si>
   <si>
@@ -215,9 +194,6 @@
     <t>4310 Pershing Ave. Se, Albuquerque, NM</t>
   </si>
   <si>
-    <t>Cooking</t>
-  </si>
-  <si>
     <t>Little Green ParkView</t>
   </si>
   <si>
@@ -227,18 +203,12 @@
     <t>821 Parkland Circle SE, Albuquerque, NM</t>
   </si>
   <si>
-    <t>Art</t>
-  </si>
-  <si>
     <t>Bill Mason</t>
   </si>
   <si>
     <t>800 Carlisle Place SE, Albuquerque, NM</t>
   </si>
   <si>
-    <t>History</t>
-  </si>
-  <si>
     <t>Esmeralda Booksworthy</t>
   </si>
   <si>
@@ -254,18 +224,12 @@
     <t>512 Jackson Street Southeast, Albuquerque, NM</t>
   </si>
   <si>
-    <t>Pet/Animal</t>
-  </si>
-  <si>
     <t>Kymberleigh's Library</t>
   </si>
   <si>
     <t>14101 Arcadia Road Ne, Albuquerque, NM</t>
   </si>
   <si>
-    <t>Non-Fiction</t>
-  </si>
-  <si>
     <t>Wells Family Library</t>
   </si>
   <si>
@@ -281,9 +245,6 @@
     <t>2913 Avenida Nevada Ne, Albuquerque, NM</t>
   </si>
   <si>
-    <t>Text/Tech Manual</t>
-  </si>
-  <si>
     <t>Laurie Lacey</t>
   </si>
   <si>
@@ -341,9 +302,6 @@
     <t>9812 Denali Road Ne, Albuquerque, NM</t>
   </si>
   <si>
-    <t>Self Improvement</t>
-  </si>
-  <si>
     <t>jackie Lyons</t>
   </si>
   <si>
@@ -567,13 +525,22 @@
   </si>
   <si>
     <t>The Ernie Pyle Library is not ADA accessible because the historic building and grounds include steps,  narrow passages,  and small spaces. The building is a 129 square foot  home built in 1940. It is a National Historic Landmark and it is on the State,  City and National registers of historic places. The closest ADA accessible Libraries include San Pedro Library,  South Broadway Library and Erna Fergusson Library.</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>Fiction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,6 +569,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -623,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -636,6 +610,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -953,63 +930,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF696C8F-C0BA-4CFB-9733-D4AF25C2BA9E}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="26.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="46.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="46.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="26.85546875" style="2"/>
+    <col min="11" max="16384" width="26.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C2" s="3" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E2" s="2" t="b">
         <v>1</v>
@@ -1021,21 +998,21 @@
         <v>-106.4979</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E3" s="2" t="b">
         <v>0</v>
@@ -1047,21 +1024,21 @@
         <v>-106.55759</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C4" s="3" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E4" s="2" t="b">
         <v>1</v>
@@ -1073,21 +1050,21 @@
         <v>-106.53207999999999</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.2">
       <c r="C5" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E5" s="2" t="b">
         <v>0</v>
@@ -1099,21 +1076,21 @@
         <v>-106.49453</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>47</v>
+        <v>159</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="E6" s="2" t="b">
         <v>1</v>
@@ -1125,21 +1102,21 @@
         <v>-106.52722</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="C7" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>0</v>
@@ -1151,21 +1128,21 @@
         <v>-106.5167993</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="C8" s="3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E8" s="2" t="b">
         <v>1</v>
@@ -1177,21 +1154,21 @@
         <v>-106.582446</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.2">
       <c r="C9" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E9" s="2" t="b">
         <v>0</v>
@@ -1203,21 +1180,21 @@
         <v>-106.5694163</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>80</v>
+        <v>159</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C10" s="3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E10" s="2" t="b">
         <v>1</v>
@@ -1229,21 +1206,21 @@
         <v>-106.55185299999999</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="C11" s="3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E11" s="2" t="b">
         <v>0</v>
@@ -1255,21 +1232,21 @@
         <v>-106.5585485</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C12" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>1</v>
@@ -1281,21 +1258,21 @@
         <v>-106.4901282</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>71</v>
+        <v>159</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C13" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E13" s="2" t="b">
         <v>0</v>
@@ -1307,21 +1284,21 @@
         <v>-106.58912599999999</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C14" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E14" s="2" t="b">
         <v>1</v>
@@ -1333,21 +1310,21 @@
         <v>-106.5931535</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="C15" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>0</v>
@@ -1359,21 +1336,21 @@
         <v>-106.6031375</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.2">
       <c r="C16" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E16" s="2" t="b">
         <v>1</v>
@@ -1385,21 +1362,21 @@
         <v>-106.60363719999999</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" ht="105" x14ac:dyDescent="0.2">
       <c r="C17" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E17" s="2" t="b">
         <v>0</v>
@@ -1411,21 +1388,21 @@
         <v>-106.59730279999999</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:10" ht="15" x14ac:dyDescent="0.2">
       <c r="C18" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E18" s="2" t="b">
         <v>1</v>
@@ -1437,21 +1414,21 @@
         <v>-106.6014539</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:10" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:10" ht="120" x14ac:dyDescent="0.2">
       <c r="C19" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E19" s="2" t="b">
         <v>0</v>
@@ -1463,21 +1440,21 @@
         <v>-106.573905</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>47</v>
+        <v>159</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C20" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E20" s="2" t="b">
         <v>1</v>
@@ -1489,21 +1466,21 @@
         <v>-106.6733902</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:10" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:10" ht="75" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E21" s="2" t="b">
         <v>1</v>
@@ -1515,21 +1492,21 @@
         <v>-106.67306859999999</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>40</v>
+        <v>159</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:10" ht="105" x14ac:dyDescent="0.2">
       <c r="C22" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E22" s="2" t="b">
         <v>1</v>
@@ -1541,21 +1518,21 @@
         <v>-106.66908359999999</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:10" ht="45" x14ac:dyDescent="0.2">
       <c r="C23" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E23" s="2" t="b">
         <v>1</v>
@@ -1567,21 +1544,21 @@
         <v>-106.6857408</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:10" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" ht="105" x14ac:dyDescent="0.2">
       <c r="C24" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E24" s="2" t="b">
         <v>1</v>
@@ -1593,21 +1570,21 @@
         <v>-106.6716868</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E25" s="2" t="b">
         <v>1</v>
@@ -1619,21 +1596,21 @@
         <v>-106.72355640000001</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:10" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" ht="75" x14ac:dyDescent="0.2">
       <c r="C26" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E26" s="2" t="b">
         <v>1</v>
@@ -1645,21 +1622,21 @@
         <v>-106.6916086</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C27" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E27" s="2" t="b">
         <v>1</v>
@@ -1671,21 +1648,21 @@
         <v>-106.6640871</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:10" ht="90" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E28" s="2" t="b">
         <v>1</v>
@@ -1697,21 +1674,21 @@
         <v>-106.70054519999999</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:10" ht="45" x14ac:dyDescent="0.2">
       <c r="C29" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E29" s="2" t="b">
         <v>1</v>
@@ -1723,21 +1700,21 @@
         <v>-106.717429</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C30" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E30" s="2" t="b">
         <v>0</v>
@@ -1749,21 +1726,21 @@
         <v>-106.7097816</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C31" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31" s="2" t="b">
         <v>1</v>
@@ -1775,21 +1752,21 @@
         <v>-106.6778819</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C32" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E32" s="2" t="b">
         <v>1</v>
@@ -1801,21 +1778,21 @@
         <v>-106.67219350000001</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C33" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E33" s="2" t="b">
         <v>0</v>
@@ -1827,21 +1804,21 @@
         <v>-106.6521122</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:10" ht="45" x14ac:dyDescent="0.2">
       <c r="C34" s="4" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E34" s="2" t="b">
         <v>0</v>
@@ -1853,21 +1830,21 @@
         <v>-106.70972</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C35" s="4" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E35" s="2" t="b">
         <v>0</v>
@@ -1879,21 +1856,21 @@
         <v>-106.72486000000001</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="3:10" ht="63.75" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" ht="75" x14ac:dyDescent="0.2">
       <c r="C36" s="4" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E36" s="2" t="b">
         <v>0</v>
@@ -1905,21 +1882,21 @@
         <v>-106.5558</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C37" s="4" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E37" s="2" t="b">
         <v>0</v>
@@ -1931,21 +1908,21 @@
         <v>-106.38930000000001</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C38" s="4" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E38" s="2" t="b">
         <v>0</v>
@@ -1957,21 +1934,21 @@
         <v>-106.58564</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="39" spans="3:10" ht="102" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" ht="105" x14ac:dyDescent="0.2">
       <c r="C39" s="4" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="E39" s="2" t="b">
         <v>0</v>
@@ -1983,21 +1960,21 @@
         <v>-106.61281</v>
       </c>
       <c r="H39" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C40" s="4" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E40" s="2" t="b">
         <v>0</v>
@@ -2009,21 +1986,21 @@
         <v>-106.56204</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="41" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" ht="45" x14ac:dyDescent="0.2">
       <c r="C41" s="4" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="E41" s="2" t="b">
         <v>0</v>
@@ -2035,21 +2012,21 @@
         <v>-106.51611</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="42" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" ht="60" x14ac:dyDescent="0.2">
       <c r="C42" s="4" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="E42" s="2" t="b">
         <v>0</v>
@@ -2061,21 +2038,21 @@
         <v>-106.49758</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C43" s="4" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="E43" s="2" t="b">
         <v>0</v>
@@ -2087,21 +2064,21 @@
         <v>-106.64831</v>
       </c>
       <c r="H43" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="J43" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="44" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C44" s="4" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="E44" s="2" t="b">
         <v>0</v>
@@ -2113,21 +2090,21 @@
         <v>-106.65331999999999</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="3:10" ht="102" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" ht="105" x14ac:dyDescent="0.2">
       <c r="C45" s="4" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E45" s="2" t="b">
         <v>0</v>
@@ -2139,21 +2116,21 @@
         <v>-106.62716</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C46" s="4" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="E46" s="2" t="b">
         <v>0</v>
@@ -2165,21 +2142,21 @@
         <v>-106.57723</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" ht="45" x14ac:dyDescent="0.2">
       <c r="C47" s="4" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E47" s="2" t="b">
         <v>0</v>
@@ -2191,21 +2168,21 @@
         <v>-106.64546</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="48" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" ht="45" x14ac:dyDescent="0.2">
       <c r="C48" s="4" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="E48" s="2" t="b">
         <v>0</v>
@@ -2217,21 +2194,21 @@
         <v>-106.68216</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="49" spans="3:10" ht="89.25" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" ht="90" x14ac:dyDescent="0.2">
       <c r="C49" s="4" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="E49" s="2" t="b">
         <v>0</v>
@@ -2243,21 +2220,21 @@
         <v>-106.64216999999999</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="50" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" ht="45" x14ac:dyDescent="0.2">
       <c r="C50" s="4" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="E50" s="2" t="b">
         <v>0</v>
@@ -2269,21 +2246,21 @@
         <v>-106.71614</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="51" spans="3:10" ht="76.5" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" ht="75" x14ac:dyDescent="0.2">
       <c r="C51" s="4" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="E51" s="2" t="b">
         <v>0</v>
@@ -2295,21 +2272,21 @@
         <v>-106.55294000000001</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="52" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" ht="45" x14ac:dyDescent="0.2">
       <c r="C52" s="4" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E52" s="2" t="b">
         <v>0</v>
@@ -2321,13 +2298,13 @@
         <v>-106.75161</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed null issue on specialization
</commit_message>
<xml_diff>
--- a/sql/library-abq-all.xlsx
+++ b/sql/library-abq-all.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nycoledavila/Desktop/DDC WEB /Git/little-library/sql/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kbowman5\little-library\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E411F3-5B0F-3E43-8D09-A842CCC270FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30279D56-23F5-469C-9479-C5D0B5BF71FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="800" windowWidth="35840" windowHeight="19500" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
+    <workbookView xWindow="7605" yWindow="5985" windowWidth="43200" windowHeight="23445" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="165">
-  <si>
-    <t>Little Library</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="163">
   <si>
     <t>La Luz</t>
   </si>
@@ -68,16 +65,10 @@
     <t>Cheryl Olsen #89915 </t>
   </si>
   <si>
-    <t>Home made library. Under a cherry tree with a bench at 2 heights for adults and children.</t>
-  </si>
-  <si>
     <t>6219 Cochiti Dr NW, Albuquerque, NM 87120</t>
   </si>
   <si>
     <t>The Road to Santiago</t>
-  </si>
-  <si>
-    <t>We carry current magazines, novels, a variety of children's books, graphic novels and more. Let our Arrow help you find the Way to El Camino. Prenez un Livre, Partagez un Livre.</t>
   </si>
   <si>
     <t>6323 Pima Place Nw, Albuquerque, NM 87120</t>
@@ -176,364 +167,367 @@
     <t>520 Dakota ST SE, Albuquerque, NM</t>
   </si>
   <si>
+    <t>Charlotte Itoh</t>
+  </si>
+  <si>
+    <t>411 Aliso Dr. Se, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Carolyn and Ken's Library &amp; Micro Pantry</t>
+  </si>
+  <si>
+    <t>Welcome neighbors, friends, and all who are not yet our friends. We hope you enjoy our Little Free Library and "Micro Pantry." We love serving as a book hub for our community, and also providing some foods and other essential items for anyone who might need a little extra help during difficult times. Our motto is "Enjoy a good read; take what you need; do a good deed." Peace to all! - Carolyn and Ken Thompson</t>
+  </si>
+  <si>
+    <t>4310 Pershing Ave. Se, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Little Green ParkView</t>
+  </si>
+  <si>
+    <t>In the 21st century when it's easy to feel disconnected, this little library brings our neighborhood together. As one of about six boxes within our area, everyone out there walking their dogs or with friends can find something to read, and talk briefly to each other as they sort through the ever-changing selections. I love to see people gathered around ours, sharing parts of their day, and their reading suggestions.</t>
+  </si>
+  <si>
+    <t>821 Parkland Circle SE, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Bill Mason</t>
+  </si>
+  <si>
+    <t>800 Carlisle Place SE, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Esmeralda Booksworthy</t>
+  </si>
+  <si>
+    <t>A place where people who love to read and people who love books can share their favorite titles</t>
+  </si>
+  <si>
+    <t>1110 Pampas Pl. Se, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Davey &amp; Jess’s Little Free Cabin Library</t>
+  </si>
+  <si>
+    <t>512 Jackson Street Southeast, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Kymberleigh's Library</t>
+  </si>
+  <si>
+    <t>14101 Arcadia Road Ne, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Wells Family Library</t>
+  </si>
+  <si>
+    <t>This library was build using 100% renewable resources and is maintained and checked regularly by our whole family! In it, you'll find all sorts of books for all ages of readers! We welcome you to visit the Wells Family Little Free Library!</t>
+  </si>
+  <si>
+    <t>8001 San Juan Road Ne, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Shirley’s Book Nook</t>
+  </si>
+  <si>
+    <t>2913 Avenida Nevada Ne, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Laurie Lacey</t>
+  </si>
+  <si>
+    <t>6910 Natalie NE, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Noah Chacon</t>
+  </si>
+  <si>
+    <t>This little library is one of 3 unanimously built as an Eagle Scout project by Noah Chacon from Troop 395, intended to spread literacy in title I school districts. Other locations of the identical libraries include Quigley and Stardust Skies park.</t>
+  </si>
+  <si>
+    <t>3107 Cuervo DR NE, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Sandia Plaza Condo's</t>
+  </si>
+  <si>
+    <t>We started collecting books since the main libraries had closed in 2020. We are a neighborhood of 101 units with all age groups. We are a thriving community of neighbors who enjoy taking part in making our community a better place.</t>
+  </si>
+  <si>
+    <t>3501 Juan Tabo Blvd Ne, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Mitchell Elementary School</t>
+  </si>
+  <si>
+    <t>The little free library was donated by a community member. Mitchell Elementary's student council decided to take charge and got the process started. We painted, dug a hole and installed the library. We thought that we could promote reading and build community relationships. We hope lots of use will come out of our effort.</t>
+  </si>
+  <si>
+    <t>10121 Comanche Ne, Albuqueruqe, NM</t>
+  </si>
+  <si>
+    <t>Blackstone Road Little Free Library</t>
+  </si>
+  <si>
+    <t>There are quite a few Little Free Libraries in Albuquerque, but none near my home. Having seen several others, I had a strong desire to put a library in my neighborhood. I mentioned it to my husband and, voila!, a library was created! Yay! It has been open for about a month. Business is good! Many new visitors each week. I'd say it is a success!</t>
+  </si>
+  <si>
+    <t>12913 Blackstone Rd Ne, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Little Free Library</t>
+  </si>
+  <si>
+    <t>We are happy to share our love of reading. Our library is on a stand at the corner of our driveway.</t>
+  </si>
+  <si>
+    <t>9812 Denali Road Ne, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>jackie Lyons</t>
+  </si>
+  <si>
+    <t>We love books and we love our community. We wanted to help join the two. That's the story.</t>
+  </si>
+  <si>
+    <t>7715 R.C. Gorman Ave NE, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>Barbara Stuecke</t>
+  </si>
+  <si>
+    <t>This Little Free Library is located in Charlie's Park in Sandia Heights at Tennyson and Cliff Rose.</t>
+  </si>
+  <si>
+    <t>2750 Cliff Rose, Albuquerque, NM</t>
+  </si>
+  <si>
+    <t>library_type</t>
+  </si>
+  <si>
+    <t>library_specialization</t>
+  </si>
+  <si>
+    <t>library_name</t>
+  </si>
+  <si>
+    <t>library_lng</t>
+  </si>
+  <si>
+    <t>library_lat</t>
+  </si>
+  <si>
+    <t>library_description</t>
+  </si>
+  <si>
+    <t>library_address</t>
+  </si>
+  <si>
+    <t>library_profile_id</t>
+  </si>
+  <si>
+    <t>library_id</t>
+  </si>
+  <si>
+    <t>6900 Gonzales SW Albuquerque NM 87121</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8081 Central NW Albuquerque NM 87121</t>
+  </si>
+  <si>
+    <t>6901 Barstow NE Albuquerque NM 87111</t>
+  </si>
+  <si>
+    <t>487 NM 333 Tijeras NM 87059</t>
+  </si>
+  <si>
+    <t>3700 San Mateo NE Albuquerque NM 87110</t>
+  </si>
+  <si>
+    <t>900 Girard SE Albuquerque NM 87106</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7601 Central Ave NE Albuquerque NM 87108</t>
+  </si>
+  <si>
+    <t>3407 Juan Tabo NE Albuquerque NM 87111</t>
+  </si>
+  <si>
+    <t>908 Eastridge NE Albuquerque NM 87123</t>
+  </si>
+  <si>
+    <t>1000 Griegos NW Albuquerque NM 87107</t>
+  </si>
+  <si>
+    <t>501 Copper NW Albuquerque NM 87102</t>
+  </si>
+  <si>
+    <t>7704-B 2nd St. NW Albuquerque NM 87107</t>
+  </si>
+  <si>
+    <t>5600 Trumbull SE Albuquerque NM 87108</t>
+  </si>
+  <si>
+    <t>1025 Broadway SE Albuquerque NM 87102</t>
+  </si>
+  <si>
+    <t>3904 Isleta SW Albuquerque NM 87105</t>
+  </si>
+  <si>
+    <t>423 Central NE Albuquerque NM 87102</t>
+  </si>
+  <si>
+    <t>5700 Bogart NW Albuquerque NM 87120</t>
+  </si>
+  <si>
+    <t>8205 Apache NE Albuquerque NM 87110</t>
+  </si>
+  <si>
+    <t>1300 Delgado SW Albuquerque NM 87121</t>
+  </si>
+  <si>
+    <t>The Alamosa Library is located in the Community Services wing of the Alamosa Center. Alamosa Center offers health,   social and recreational services provided by other City agencies.</t>
+  </si>
+  <si>
+    <t>The Central and Unser Library is located on Central Ave just west of Unser Blvd,  next to the Central Unser Transit Station.</t>
+  </si>
+  <si>
+    <t>The Cherry Hills Library is located at the corner of Harper Road and Barstow Street NE,  one block east of the intersection of Harper Road and Wyoming Blvd. The Library is adjacent to the Del Norte Shopping Center whose tenants include McDonald's and Walgreens.</t>
+  </si>
+  <si>
+    <t>The East Mountain Library is located midway along Tijeras Canyon,  just adjacent to Exit 175 off of I-40.</t>
+  </si>
+  <si>
+    <t>The Erna Fergusson Library is located on the east side of San Mateo Blvd between Comanche Rd and Montgomery Blvd.</t>
+  </si>
+  <si>
+    <t>The International District Library is located on Central Ave just east of Louisiana Blvd,  on the corner of Central and San Pablo St. NE.</t>
+  </si>
+  <si>
+    <t>The Juan Tabo Library is located on Juan Tabo Blvd,  halfway between Candelaria Road and Comanche Road,  on the west side of the street. Note the building is set back off the street.</t>
+  </si>
+  <si>
+    <t>The Lomas Tramway Library is located on the southwest corner of Lomas Blvd and Tramway Blvd. Note that there is no access from Tramway. The parking lot entrance is on Eastridge Drive,  which runs parallel to Tramway.</t>
+  </si>
+  <si>
+    <t>The Los Griegos Library is located on the southwest corner of 10th Street and Griegos Road in a residential neighborhood.</t>
+  </si>
+  <si>
+    <t>Main Library is in downtown Albuquerque on Copper Avenue NW,  between 5th and 6th streets.</t>
+  </si>
+  <si>
+    <t>The Rudolfo Anaya North Valley Library is located at 7704 2nd St. NW on the east side of 2nd Street,  approximately 9/10 of a mile north of Osuna Blvd and approximately 9/10 of a mile south of Paseo del Norte.  The Library is next to First Choice Community Healthcare and shares the incoming parking lot entrance with the Center.  The front entrances of the Library faces the parking lot rather than 2nd Street.</t>
+  </si>
+  <si>
+    <t>The San Pedro Library is located in a residential area on the SW corner of San Pedro Drive and Trumbull SE.</t>
+  </si>
+  <si>
+    <t>The South Broadway Library shares the building at 1025 Broadway SE with the South Broadway Cultural Center. The large sign outside the building serves as a marquee for the Cultural Center.</t>
+  </si>
+  <si>
+    <t>The South Valley Library is located one-quarter mile south of the intersection of Rio Bravo Blvd. and Isleta Blvd SW. The Library is at the intersection of Isleta Blvd. and Camino del Valle.</t>
+  </si>
+  <si>
+    <t>The Special Collections Library of the Public Library houses research collections on Albuquerque history and New Mexico history and culture. The 1925 Pueblo/Spanish Revival-style building is a registered Albuquerque landmark in the historic Huning Highlands neighborhood. The research collections are available for in house use only.</t>
+  </si>
+  <si>
+    <t>The Taylor Ranch Library is located one block west of Unser Blvd and two blocks south of Montano Road in a residential neighborhood in the Santa Fe Village Park.</t>
+  </si>
+  <si>
+    <t>The Tony Hillerman Library (formerly the Wyoming Library) is located behind the Hoffmantown Shopping Center at the intersection of Wyoming Blvd and Menaul Blvd. on Apache Street NE. It is on a separate,  irregularly shaped block with beautiful public rose gardens on each end adjoining the parking lots.</t>
+  </si>
+  <si>
+    <t>The Westgate Heights Library is located just south of Carlos Rey Elementary School in the NW corner of Carlos Rey Park. We share our parking lot with the Carlos Rey Child Development Center.</t>
+  </si>
+  <si>
+    <t>Alamosa Library</t>
+  </si>
+  <si>
+    <t>Central and Unser Library</t>
+  </si>
+  <si>
+    <t>Cherry Hills Library</t>
+  </si>
+  <si>
+    <t>East Mountain Library</t>
+  </si>
+  <si>
+    <t>Erna Fergusson Library</t>
+  </si>
+  <si>
+    <t>Ernie Pyle Library</t>
+  </si>
+  <si>
+    <t>International District Library</t>
+  </si>
+  <si>
+    <t>Juan Tabo Library</t>
+  </si>
+  <si>
+    <t>Lomas Tramway Library</t>
+  </si>
+  <si>
+    <t>Los Griegos Library</t>
+  </si>
+  <si>
+    <t>Main Library</t>
+  </si>
+  <si>
+    <t>Rudolfo Anaya North Valley Library</t>
+  </si>
+  <si>
+    <t>San Pedro Library</t>
+  </si>
+  <si>
+    <t>South Broadway Library</t>
+  </si>
+  <si>
+    <t>South Valley Library</t>
+  </si>
+  <si>
+    <t>Special Collections Library</t>
+  </si>
+  <si>
+    <t>Taylor Ranch Library</t>
+  </si>
+  <si>
+    <t>Tony Hillerman Library</t>
+  </si>
+  <si>
+    <t>Westgate Heights Library</t>
+  </si>
+  <si>
+    <t>library_event_opt_in</t>
+  </si>
+  <si>
+    <t>The Ernie Pyle Library is not ADA accessible because the historic building and grounds include steps,  narrow passages,  and small spaces. The building is a 129 square foot  home built in 1940. It is a National Historic Landmark and it is on the State,  City and National registers of historic places. The closest ADA accessible Libraries include San Pedro Library,  South Broadway Library and Erna Fergusson Library.</t>
+  </si>
+  <si>
+    <t>Public Library</t>
+  </si>
+  <si>
+    <t>Little Library</t>
+  </si>
+  <si>
+    <t>Our Little Free Library is located outside Cleveland Middle School where I was a teacher-librarian for 18 years. At my retirement in May 2017, I wanted to leave something for my community that would promote reading and literacy so what could be more perfect! The endeavor was a family effort with my son-in-law making the library, my husband painting it and my daughter and grandChildren supplying books.It is my fervent wish that the Cleveland community will enjoy there library for many happy years</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>We carry current magazines, novels, a variety of Children's books, graphic novels and more. Let our Arrow help you find the Way to El Camino. Prenez un Livre, Partagez un Livre.</t>
+  </si>
+  <si>
+    <t>Home made library. Under a cherry tree with a bench at 2 heights for adults and Children.</t>
+  </si>
+  <si>
+    <t>Fiction</t>
+  </si>
+  <si>
     <t>Romance</t>
   </si>
   <si>
-    <t>Charlotte Itoh</t>
-  </si>
-  <si>
-    <t>411 Aliso Dr. Se, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Carolyn and Ken's Library &amp; Micro Pantry</t>
-  </si>
-  <si>
-    <t>Welcome neighbors, friends, and all who are not yet our friends. We hope you enjoy our Little Free Library and "Micro Pantry." We love serving as a book hub for our community, and also providing some foods and other essential items for anyone who might need a little extra help during difficult times. Our motto is "Enjoy a good read; take what you need; do a good deed." Peace to all! - Carolyn and Ken Thompson</t>
-  </si>
-  <si>
-    <t>4310 Pershing Ave. Se, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Little Green ParkView</t>
-  </si>
-  <si>
-    <t>In the 21st century when it's easy to feel disconnected, this little library brings our neighborhood together. As one of about six boxes within our area, everyone out there walking their dogs or with friends can find something to read, and talk briefly to each other as they sort through the ever-changing selections. I love to see people gathered around ours, sharing parts of their day, and their reading suggestions.</t>
-  </si>
-  <si>
-    <t>821 Parkland Circle SE, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Bill Mason</t>
-  </si>
-  <si>
-    <t>800 Carlisle Place SE, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Esmeralda Booksworthy</t>
-  </si>
-  <si>
-    <t>A place where people who love to read and people who love books can share their favorite titles</t>
-  </si>
-  <si>
-    <t>1110 Pampas Pl. Se, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Davey &amp; Jess’s Little Free Cabin Library</t>
-  </si>
-  <si>
-    <t>512 Jackson Street Southeast, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Kymberleigh's Library</t>
-  </si>
-  <si>
-    <t>14101 Arcadia Road Ne, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Wells Family Library</t>
-  </si>
-  <si>
-    <t>This library was build using 100% renewable resources and is maintained and checked regularly by our whole family! In it, you'll find all sorts of books for all ages of readers! We welcome you to visit the Wells Family Little Free Library!</t>
-  </si>
-  <si>
-    <t>8001 San Juan Road Ne, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Shirley’s Book Nook</t>
-  </si>
-  <si>
-    <t>2913 Avenida Nevada Ne, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Laurie Lacey</t>
-  </si>
-  <si>
-    <t>Our Little Free Library is located outside Cleveland Middle School where I was a teacher-librarian for 18 years. At my retirement in May 2017, I wanted to leave something for my community that would promote reading and literacy so what could be more perfect! The endeavor was a family effort with my son-in-law making the library, my husband painting it and my daughter and grandchildren supplying books.It is my fervent wish that the Cleveland community will enjoy there library for many happy years</t>
-  </si>
-  <si>
-    <t>6910 Natalie NE, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Noah Chacon</t>
-  </si>
-  <si>
-    <t>This little library is one of 3 unanimously built as an Eagle Scout project by Noah Chacon from Troop 395, intended to spread literacy in title I school districts. Other locations of the identical libraries include Quigley and Stardust Skies park.</t>
-  </si>
-  <si>
-    <t>3107 Cuervo DR NE, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Sandia Plaza Condo's</t>
-  </si>
-  <si>
-    <t>We started collecting books since the main libraries had closed in 2020. We are a neighborhood of 101 units with all age groups. We are a thriving community of neighbors who enjoy taking part in making our community a better place.</t>
-  </si>
-  <si>
-    <t>3501 Juan Tabo Blvd Ne, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Home Imporovement</t>
-  </si>
-  <si>
-    <t>Mitchell Elementary School</t>
-  </si>
-  <si>
-    <t>The little free library was donated by a community member. Mitchell Elementary's student council decided to take charge and got the process started. We painted, dug a hole and installed the library. We thought that we could promote reading and build community relationships. We hope lots of use will come out of our effort.</t>
-  </si>
-  <si>
-    <t>10121 Comanche Ne, Albuqueruqe, NM</t>
-  </si>
-  <si>
-    <t>Blackstone Road Little Free Library</t>
-  </si>
-  <si>
-    <t>There are quite a few Little Free Libraries in Albuquerque, but none near my home. Having seen several others, I had a strong desire to put a library in my neighborhood. I mentioned it to my husband and, voila!, a library was created! Yay! It has been open for about a month. Business is good! Many new visitors each week. I'd say it is a success!</t>
-  </si>
-  <si>
-    <t>12913 Blackstone Rd Ne, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Little Free Library</t>
-  </si>
-  <si>
-    <t>We are happy to share our love of reading. Our library is on a stand at the corner of our driveway.</t>
-  </si>
-  <si>
-    <t>9812 Denali Road Ne, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>jackie Lyons</t>
-  </si>
-  <si>
-    <t>We love books and we love our community. We wanted to help join the two. That's the story.</t>
-  </si>
-  <si>
-    <t>7715 R.C. Gorman Ave NE, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>Barbara Stuecke</t>
-  </si>
-  <si>
-    <t>This Little Free Library is located in Charlie's Park in Sandia Heights at Tennyson and Cliff Rose.</t>
-  </si>
-  <si>
-    <t>2750 Cliff Rose, Albuquerque, NM</t>
-  </si>
-  <si>
-    <t>library_type</t>
-  </si>
-  <si>
-    <t>library_specialization</t>
-  </si>
-  <si>
-    <t>library_name</t>
-  </si>
-  <si>
-    <t>library_lng</t>
-  </si>
-  <si>
-    <t>library_lat</t>
-  </si>
-  <si>
-    <t>library_description</t>
-  </si>
-  <si>
-    <t>library_address</t>
-  </si>
-  <si>
-    <t>library_profile_id</t>
-  </si>
-  <si>
-    <t>library_id</t>
-  </si>
-  <si>
-    <t>6900 Gonzales SW Albuquerque NM 87121</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8081 Central NW Albuquerque NM 87121</t>
-  </si>
-  <si>
-    <t>6901 Barstow NE Albuquerque NM 87111</t>
-  </si>
-  <si>
-    <t>487 NM 333 Tijeras NM 87059</t>
-  </si>
-  <si>
-    <t>3700 San Mateo NE Albuquerque NM 87110</t>
-  </si>
-  <si>
-    <t>900 Girard SE Albuquerque NM 87106</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7601 Central Ave NE Albuquerque NM 87108</t>
-  </si>
-  <si>
-    <t>3407 Juan Tabo NE Albuquerque NM 87111</t>
-  </si>
-  <si>
-    <t>908 Eastridge NE Albuquerque NM 87123</t>
-  </si>
-  <si>
-    <t>1000 Griegos NW Albuquerque NM 87107</t>
-  </si>
-  <si>
-    <t>501 Copper NW Albuquerque NM 87102</t>
-  </si>
-  <si>
-    <t>7704-B 2nd St. NW Albuquerque NM 87107</t>
-  </si>
-  <si>
-    <t>5600 Trumbull SE Albuquerque NM 87108</t>
-  </si>
-  <si>
-    <t>1025 Broadway SE Albuquerque NM 87102</t>
-  </si>
-  <si>
-    <t>3904 Isleta SW Albuquerque NM 87105</t>
-  </si>
-  <si>
-    <t>423 Central NE Albuquerque NM 87102</t>
-  </si>
-  <si>
-    <t>5700 Bogart NW Albuquerque NM 87120</t>
-  </si>
-  <si>
-    <t>8205 Apache NE Albuquerque NM 87110</t>
-  </si>
-  <si>
-    <t>1300 Delgado SW Albuquerque NM 87121</t>
-  </si>
-  <si>
-    <t>The Alamosa Library is located in the Community Services wing of the Alamosa Center. Alamosa Center offers health,   social and recreational services provided by other City agencies.</t>
-  </si>
-  <si>
-    <t>The Central and Unser Library is located on Central Ave just west of Unser Blvd,  next to the Central Unser Transit Station.</t>
-  </si>
-  <si>
-    <t>The Cherry Hills Library is located at the corner of Harper Road and Barstow Street NE,  one block east of the intersection of Harper Road and Wyoming Blvd. The Library is adjacent to the Del Norte Shopping Center whose tenants include McDonald's and Walgreens.</t>
-  </si>
-  <si>
-    <t>The East Mountain Library is located midway along Tijeras Canyon,  just adjacent to Exit 175 off of I-40.</t>
-  </si>
-  <si>
-    <t>The Erna Fergusson Library is located on the east side of San Mateo Blvd between Comanche Rd and Montgomery Blvd.</t>
-  </si>
-  <si>
-    <t>The International District Library is located on Central Ave just east of Louisiana Blvd,  on the corner of Central and San Pablo St. NE.</t>
-  </si>
-  <si>
-    <t>The Juan Tabo Library is located on Juan Tabo Blvd,  halfway between Candelaria Road and Comanche Road,  on the west side of the street. Note the building is set back off the street.</t>
-  </si>
-  <si>
-    <t>The Lomas Tramway Library is located on the southwest corner of Lomas Blvd and Tramway Blvd. Note that there is no access from Tramway. The parking lot entrance is on Eastridge Drive,  which runs parallel to Tramway.</t>
-  </si>
-  <si>
-    <t>The Los Griegos Library is located on the southwest corner of 10th Street and Griegos Road in a residential neighborhood.</t>
-  </si>
-  <si>
-    <t>Main Library is in downtown Albuquerque on Copper Avenue NW,  between 5th and 6th streets.</t>
-  </si>
-  <si>
-    <t>The Rudolfo Anaya North Valley Library is located at 7704 2nd St. NW on the east side of 2nd Street,  approximately 9/10 of a mile north of Osuna Blvd and approximately 9/10 of a mile south of Paseo del Norte.  The Library is next to First Choice Community Healthcare and shares the incoming parking lot entrance with the Center.  The front entrances of the Library faces the parking lot rather than 2nd Street.</t>
-  </si>
-  <si>
-    <t>The San Pedro Library is located in a residential area on the SW corner of San Pedro Drive and Trumbull SE.</t>
-  </si>
-  <si>
-    <t>The South Broadway Library shares the building at 1025 Broadway SE with the South Broadway Cultural Center. The large sign outside the building serves as a marquee for the Cultural Center.</t>
-  </si>
-  <si>
-    <t>The South Valley Library is located one-quarter mile south of the intersection of Rio Bravo Blvd. and Isleta Blvd SW. The Library is at the intersection of Isleta Blvd. and Camino del Valle.</t>
-  </si>
-  <si>
-    <t>The Special Collections Library of the Public Library houses research collections on Albuquerque history and New Mexico history and culture. The 1925 Pueblo/Spanish Revival-style building is a registered Albuquerque landmark in the historic Huning Highlands neighborhood. The research collections are available for in house use only.</t>
-  </si>
-  <si>
-    <t>The Taylor Ranch Library is located one block west of Unser Blvd and two blocks south of Montano Road in a residential neighborhood in the Santa Fe Village Park.</t>
-  </si>
-  <si>
-    <t>The Tony Hillerman Library (formerly the Wyoming Library) is located behind the Hoffmantown Shopping Center at the intersection of Wyoming Blvd and Menaul Blvd. on Apache Street NE. It is on a separate,  irregularly shaped block with beautiful public rose gardens on each end adjoining the parking lots.</t>
-  </si>
-  <si>
-    <t>The Westgate Heights Library is located just south of Carlos Rey Elementary School in the NW corner of Carlos Rey Park. We share our parking lot with the Carlos Rey Child Development Center.</t>
-  </si>
-  <si>
-    <t>Alamosa Library</t>
-  </si>
-  <si>
-    <t>Central and Unser Library</t>
-  </si>
-  <si>
-    <t>Cherry Hills Library</t>
-  </si>
-  <si>
-    <t>East Mountain Library</t>
-  </si>
-  <si>
-    <t>Erna Fergusson Library</t>
-  </si>
-  <si>
-    <t>Ernie Pyle Library</t>
-  </si>
-  <si>
-    <t>International District Library</t>
-  </si>
-  <si>
-    <t>Juan Tabo Library</t>
-  </si>
-  <si>
-    <t>Lomas Tramway Library</t>
-  </si>
-  <si>
-    <t>Los Griegos Library</t>
-  </si>
-  <si>
-    <t>Main Library</t>
-  </si>
-  <si>
-    <t>Rudolfo Anaya North Valley Library</t>
-  </si>
-  <si>
-    <t>San Pedro Library</t>
-  </si>
-  <si>
-    <t>South Broadway Library</t>
-  </si>
-  <si>
-    <t>South Valley Library</t>
-  </si>
-  <si>
-    <t>Special Collections Library</t>
-  </si>
-  <si>
-    <t>Taylor Ranch Library</t>
-  </si>
-  <si>
-    <t>Tony Hillerman Library</t>
-  </si>
-  <si>
-    <t>Westgate Heights Library</t>
-  </si>
-  <si>
-    <t>Public Library</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>library_event_opt_in</t>
-  </si>
-  <si>
-    <t>The Ernie Pyle Library is not ADA accessible because the historic building and grounds include steps,  narrow passages,  and small spaces. The building is a 129 square foot  home built in 1940. It is a National Historic Landmark and it is on the State,  City and National registers of historic places. The closest ADA accessible Libraries include San Pedro Library,  South Broadway Library and Erna Fergusson Library.</t>
-  </si>
-  <si>
-    <t>Public</t>
-  </si>
-  <si>
-    <t>Children</t>
-  </si>
-  <si>
-    <t>Fiction</t>
+    <t>Home Improvement</t>
   </si>
 </sst>
 </file>
@@ -930,63 +924,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF696C8F-C0BA-4CFB-9733-D4AF25C2BA9E}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="26.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="26.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="46.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="26.83203125" style="2"/>
+    <col min="11" max="16384" width="26.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E2" s="2" t="b">
         <v>1</v>
@@ -998,21 +992,21 @@
         <v>-106.4979</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E3" s="2" t="b">
         <v>0</v>
@@ -1024,21 +1018,21 @@
         <v>-106.55759</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E4" s="2" t="b">
         <v>1</v>
@@ -1050,21 +1044,21 @@
         <v>-106.53207999999999</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E5" s="2" t="b">
         <v>0</v>
@@ -1076,21 +1070,21 @@
         <v>-106.49453</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E6" s="2" t="b">
         <v>1</v>
@@ -1102,21 +1096,21 @@
         <v>-106.52722</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>0</v>
@@ -1128,21 +1122,21 @@
         <v>-106.5167993</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E8" s="2" t="b">
         <v>1</v>
@@ -1154,21 +1148,21 @@
         <v>-106.582446</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="E9" s="2" t="b">
         <v>0</v>
@@ -1180,21 +1174,18 @@
         <v>-106.5694163</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>159</v>
+        <v>63</v>
       </c>
       <c r="E10" s="2" t="b">
         <v>1</v>
@@ -1206,21 +1197,21 @@
         <v>-106.55185299999999</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E11" s="2" t="b">
         <v>0</v>
@@ -1232,21 +1223,18 @@
         <v>-106.5585485</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>159</v>
+        <v>58</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>1</v>
@@ -1258,21 +1246,18 @@
         <v>-106.4901282</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>159</v>
+        <v>56</v>
       </c>
       <c r="E13" s="2" t="b">
         <v>0</v>
@@ -1284,21 +1269,21 @@
         <v>-106.58912599999999</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E14" s="2" t="b">
         <v>1</v>
@@ -1310,21 +1295,18 @@
         <v>-106.5931535</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>0</v>
@@ -1336,21 +1318,21 @@
         <v>-106.6031375</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="105" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="102" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E16" s="2" t="b">
         <v>1</v>
@@ -1362,21 +1344,21 @@
         <v>-106.60363719999999</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10" ht="105" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" ht="102" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E17" s="2" t="b">
         <v>0</v>
@@ -1388,21 +1370,18 @@
         <v>-106.59730279999999</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" ht="15" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>159</v>
+        <v>43</v>
       </c>
       <c r="E18" s="2" t="b">
         <v>1</v>
@@ -1414,21 +1393,21 @@
         <v>-106.6014539</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:10" ht="120" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" ht="127.5" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E19" s="2" t="b">
         <v>0</v>
@@ -1440,21 +1419,21 @@
         <v>-106.573905</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E20" s="2" t="b">
         <v>1</v>
@@ -1466,21 +1445,21 @@
         <v>-106.6733902</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="3:10" ht="75" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E21" s="2" t="b">
         <v>1</v>
@@ -1492,21 +1471,21 @@
         <v>-106.67306859999999</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="3:10" ht="105" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" ht="102" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E22" s="2" t="b">
         <v>1</v>
@@ -1518,21 +1497,21 @@
         <v>-106.66908359999999</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" ht="45" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E23" s="2" t="b">
         <v>1</v>
@@ -1544,21 +1523,21 @@
         <v>-106.6857408</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" ht="105" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" ht="114.75" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E24" s="2" t="b">
         <v>1</v>
@@ -1570,21 +1549,21 @@
         <v>-106.6716868</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E25" s="2" t="b">
         <v>1</v>
@@ -1596,21 +1575,21 @@
         <v>-106.72355640000001</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:10" ht="75" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E26" s="2" t="b">
         <v>1</v>
@@ -1622,21 +1601,21 @@
         <v>-106.6916086</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E27" s="2" t="b">
         <v>1</v>
@@ -1648,21 +1627,21 @@
         <v>-106.6640871</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:10" ht="90" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" ht="102" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E28" s="2" t="b">
         <v>1</v>
@@ -1674,21 +1653,21 @@
         <v>-106.70054519999999</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="3:10" ht="45" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" ht="51" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="E29" s="2" t="b">
         <v>1</v>
@@ -1700,21 +1679,21 @@
         <v>-106.717429</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>10</v>
+        <v>159</v>
       </c>
       <c r="E30" s="2" t="b">
         <v>0</v>
@@ -1726,21 +1705,21 @@
         <v>-106.7097816</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E31" s="2" t="b">
         <v>1</v>
@@ -1752,21 +1731,18 @@
         <v>-106.6778819</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>159</v>
+        <v>4</v>
       </c>
       <c r="E32" s="2" t="b">
         <v>1</v>
@@ -1778,21 +1754,21 @@
         <v>-106.67219350000001</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="2" t="b">
         <v>0</v>
@@ -1804,21 +1780,21 @@
         <v>-106.6521122</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" ht="45" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" ht="51" x14ac:dyDescent="0.2">
       <c r="C34" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E34" s="2" t="b">
         <v>0</v>
@@ -1830,21 +1806,21 @@
         <v>-106.70972</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C35" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E35" s="2" t="b">
         <v>0</v>
@@ -1856,21 +1832,21 @@
         <v>-106.72486000000001</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="36" spans="3:10" ht="75" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C36" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E36" s="2" t="b">
         <v>0</v>
@@ -1882,21 +1858,21 @@
         <v>-106.5558</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C37" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E37" s="2" t="b">
         <v>0</v>
@@ -1908,21 +1884,21 @@
         <v>-106.38930000000001</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C38" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E38" s="2" t="b">
         <v>0</v>
@@ -1934,21 +1910,21 @@
         <v>-106.58564</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="3:10" ht="105" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" ht="102" x14ac:dyDescent="0.2">
       <c r="C39" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E39" s="2" t="b">
         <v>0</v>
@@ -1960,21 +1936,21 @@
         <v>-106.61281</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C40" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E40" s="2" t="b">
         <v>0</v>
@@ -1986,21 +1962,21 @@
         <v>-106.56204</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="3:10" ht="45" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" ht="51" x14ac:dyDescent="0.2">
       <c r="C41" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E41" s="2" t="b">
         <v>0</v>
@@ -2012,21 +1988,21 @@
         <v>-106.51611</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="3:10" ht="60" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" ht="51" x14ac:dyDescent="0.2">
       <c r="C42" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E42" s="2" t="b">
         <v>0</v>
@@ -2038,21 +2014,21 @@
         <v>-106.49758</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="43" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C43" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E43" s="2" t="b">
         <v>0</v>
@@ -2064,21 +2040,21 @@
         <v>-106.64831</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="44" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C44" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E44" s="2" t="b">
         <v>0</v>
@@ -2090,21 +2066,21 @@
         <v>-106.65331999999999</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="3:10" ht="105" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" ht="102" x14ac:dyDescent="0.2">
       <c r="C45" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E45" s="2" t="b">
         <v>0</v>
@@ -2116,21 +2092,21 @@
         <v>-106.62716</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="3:10" ht="30" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C46" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E46" s="2" t="b">
         <v>0</v>
@@ -2142,21 +2118,21 @@
         <v>-106.57723</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="3:10" ht="45" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" ht="51" x14ac:dyDescent="0.2">
       <c r="C47" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E47" s="2" t="b">
         <v>0</v>
@@ -2168,21 +2144,21 @@
         <v>-106.64546</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="3:10" ht="45" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" ht="51" x14ac:dyDescent="0.2">
       <c r="C48" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E48" s="2" t="b">
         <v>0</v>
@@ -2194,21 +2170,21 @@
         <v>-106.68216</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="49" spans="3:10" ht="90" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" ht="89.25" x14ac:dyDescent="0.2">
       <c r="C49" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E49" s="2" t="b">
         <v>0</v>
@@ -2220,21 +2196,21 @@
         <v>-106.64216999999999</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="50" spans="3:10" ht="45" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C50" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E50" s="2" t="b">
         <v>0</v>
@@ -2246,21 +2222,21 @@
         <v>-106.71614</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="51" spans="3:10" ht="75" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="C51" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E51" s="2" t="b">
         <v>0</v>
@@ -2272,21 +2248,21 @@
         <v>-106.55294000000001</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="52" spans="3:10" ht="45" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" ht="51" x14ac:dyDescent="0.2">
       <c r="C52" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E52" s="2" t="b">
         <v>0</v>
@@ -2298,13 +2274,13 @@
         <v>-106.75161</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed up pins and drop down spec menu
</commit_message>
<xml_diff>
--- a/sql/library-abq-all.xlsx
+++ b/sql/library-abq-all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kbowman5\little-library\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30279D56-23F5-469C-9479-C5D0B5BF71FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139062E5-DEA9-477C-A24C-97CEC21816C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7605" yWindow="5985" windowWidth="43200" windowHeight="23445" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
+    <workbookView xWindow="6435" yWindow="1470" windowWidth="29775" windowHeight="19245" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="183">
   <si>
     <t>La Luz</t>
   </si>
@@ -528,6 +528,66 @@
   </si>
   <si>
     <t>Home Improvement</t>
+  </si>
+  <si>
+    <t>Animals or Pets</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Automotive</t>
+  </si>
+  <si>
+    <t>Baby</t>
+  </si>
+  <si>
+    <t>Cooking</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Fitness</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Horror</t>
+  </si>
+  <si>
+    <t>Nature</t>
+  </si>
+  <si>
+    <t>Religious</t>
+  </si>
+  <si>
+    <t>Satire</t>
+  </si>
+  <si>
+    <t>Science Fiction</t>
+  </si>
+  <si>
+    <t>Self Improvement</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>Young Adults</t>
+  </si>
+  <si>
+    <t>Technical or Textbooks</t>
+  </si>
+  <si>
+    <t>Official Community</t>
   </si>
 </sst>
 </file>
@@ -924,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF696C8F-C0BA-4CFB-9733-D4AF25C2BA9E}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1021,7 +1081,7 @@
         <v>81</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>155</v>
@@ -1047,7 +1107,7 @@
         <v>78</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>155</v>
@@ -1073,7 +1133,7 @@
         <v>75</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>155</v>
@@ -1099,7 +1159,7 @@
         <v>72</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>155</v>
@@ -1125,7 +1185,7 @@
         <v>69</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>155</v>
@@ -1151,7 +1211,7 @@
         <v>66</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>155</v>
@@ -1177,7 +1237,7 @@
         <v>64</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>155</v>
@@ -1200,7 +1260,7 @@
         <v>62</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>155</v>
@@ -1226,7 +1286,7 @@
         <v>59</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>155</v>
@@ -1249,7 +1309,7 @@
         <v>57</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>155</v>
@@ -1272,7 +1332,7 @@
         <v>55</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>155</v>
@@ -1298,7 +1358,7 @@
         <v>52</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>155</v>
@@ -1321,7 +1381,7 @@
         <v>50</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>155</v>
@@ -1346,9 +1406,6 @@
       <c r="H16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="J16" s="2" t="s">
         <v>155</v>
       </c>
@@ -1372,9 +1429,6 @@
       <c r="H17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="J17" s="2" t="s">
         <v>155</v>
       </c>
@@ -1396,7 +1450,7 @@
         <v>42</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>155</v>
@@ -1422,7 +1476,7 @@
         <v>39</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>155</v>
@@ -1448,7 +1502,7 @@
         <v>36</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>155</v>
@@ -1474,7 +1528,7 @@
         <v>33</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>155</v>
@@ -1500,7 +1554,7 @@
         <v>30</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>155</v>
@@ -1526,7 +1580,7 @@
         <v>27</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>155</v>
@@ -1552,7 +1606,7 @@
         <v>24</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>155</v>
@@ -1578,7 +1632,7 @@
         <v>21</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>155</v>
@@ -1604,7 +1658,7 @@
         <v>18</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>155</v>
@@ -1630,7 +1684,7 @@
         <v>15</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>155</v>
@@ -1655,9 +1709,6 @@
       <c r="H28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="J28" s="2" t="s">
         <v>155</v>
       </c>
@@ -1681,9 +1732,7 @@
       <c r="H29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I29" s="5" t="s">
-        <v>162</v>
-      </c>
+      <c r="I29" s="5"/>
       <c r="J29" s="2" t="s">
         <v>155</v>
       </c>
@@ -1707,9 +1756,6 @@
       <c r="H30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="J30" s="2" t="s">
         <v>155</v>
       </c>
@@ -1733,9 +1779,6 @@
       <c r="H31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="J31" s="2" t="s">
         <v>155</v>
       </c>
@@ -1756,9 +1799,6 @@
       <c r="H32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="J32" s="2" t="s">
         <v>155</v>
       </c>
@@ -1782,9 +1822,6 @@
       <c r="H33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="J33" s="2" t="s">
         <v>155</v>
       </c>
@@ -1809,7 +1846,7 @@
         <v>133</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>154</v>
@@ -1835,7 +1872,7 @@
         <v>134</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>154</v>
@@ -1861,7 +1898,7 @@
         <v>135</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>154</v>
@@ -1887,7 +1924,7 @@
         <v>136</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>154</v>
@@ -1913,7 +1950,7 @@
         <v>137</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>154</v>
@@ -1939,7 +1976,7 @@
         <v>138</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>154</v>
@@ -1965,7 +2002,7 @@
         <v>139</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>154</v>
@@ -1991,7 +2028,7 @@
         <v>140</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>154</v>
@@ -2017,7 +2054,7 @@
         <v>141</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>154</v>
@@ -2043,7 +2080,7 @@
         <v>142</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>154</v>
@@ -2069,7 +2106,7 @@
         <v>143</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>154</v>
@@ -2095,7 +2132,7 @@
         <v>144</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>154</v>
@@ -2121,7 +2158,7 @@
         <v>145</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>154</v>
@@ -2147,7 +2184,7 @@
         <v>146</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>154</v>
@@ -2173,7 +2210,7 @@
         <v>147</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>154</v>
@@ -2199,7 +2236,7 @@
         <v>148</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>154</v>
@@ -2225,7 +2262,7 @@
         <v>149</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>154</v>
@@ -2251,7 +2288,7 @@
         <v>150</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>154</v>
@@ -2277,7 +2314,7 @@
         <v>151</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>154</v>

</xml_diff>

<commit_message>
changed PostgreSQL file slightly to fit prior push to Library Spec dropdown
</commit_message>
<xml_diff>
--- a/sql/library-abq-all.xlsx
+++ b/sql/library-abq-all.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kbowman5\little-library\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139062E5-DEA9-477C-A24C-97CEC21816C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{93581B98-C45A-4122-87D5-3BEB52B2CBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6435" yWindow="1470" windowWidth="29775" windowHeight="19245" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="library-abq-all" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="182">
   <si>
     <t>La Luz</t>
   </si>
@@ -569,9 +569,6 @@
     <t>Satire</t>
   </si>
   <si>
-    <t>Science Fiction</t>
-  </si>
-  <si>
     <t>Self Improvement</t>
   </si>
   <si>
@@ -581,13 +578,13 @@
     <t>Sports</t>
   </si>
   <si>
-    <t>Young Adults</t>
-  </si>
-  <si>
     <t>Technical or Textbooks</t>
   </si>
   <si>
     <t>Official Community</t>
+  </si>
+  <si>
+    <t>Young Adult</t>
   </si>
 </sst>
 </file>
@@ -984,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF696C8F-C0BA-4CFB-9733-D4AF25C2BA9E}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1054,9 +1051,6 @@
       <c r="H2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="J2" s="2" t="s">
         <v>155</v>
       </c>
@@ -1553,9 +1547,6 @@
       <c r="H22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>176</v>
-      </c>
       <c r="J22" s="2" t="s">
         <v>155</v>
       </c>
@@ -1580,7 +1571,7 @@
         <v>27</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>155</v>
@@ -1606,7 +1597,7 @@
         <v>24</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>155</v>
@@ -1632,7 +1623,7 @@
         <v>21</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>155</v>
@@ -1658,7 +1649,7 @@
         <v>18</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>155</v>
@@ -1684,7 +1675,7 @@
         <v>15</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>155</v>
@@ -1846,7 +1837,7 @@
         <v>133</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>154</v>
@@ -1872,7 +1863,7 @@
         <v>134</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>154</v>
@@ -1898,7 +1889,7 @@
         <v>135</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>154</v>
@@ -1924,7 +1915,7 @@
         <v>136</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>154</v>
@@ -1950,7 +1941,7 @@
         <v>137</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>154</v>
@@ -1976,7 +1967,7 @@
         <v>138</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>154</v>
@@ -2002,7 +1993,7 @@
         <v>139</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>154</v>
@@ -2028,7 +2019,7 @@
         <v>140</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>154</v>
@@ -2054,7 +2045,7 @@
         <v>141</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>154</v>
@@ -2080,7 +2071,7 @@
         <v>142</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>154</v>
@@ -2106,7 +2097,7 @@
         <v>143</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>154</v>
@@ -2132,7 +2123,7 @@
         <v>144</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>154</v>
@@ -2158,7 +2149,7 @@
         <v>145</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>154</v>
@@ -2184,7 +2175,7 @@
         <v>146</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>154</v>
@@ -2210,7 +2201,7 @@
         <v>147</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>154</v>
@@ -2236,7 +2227,7 @@
         <v>148</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>154</v>
@@ -2262,7 +2253,7 @@
         <v>149</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>154</v>
@@ -2288,7 +2279,7 @@
         <v>150</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>154</v>
@@ -2314,7 +2305,7 @@
         <v>151</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>154</v>

</xml_diff>

<commit_message>
got as far as I can and found out I have to use PostgreSQL Inner JOIN to make this happen. Going to seperate branch to work that
</commit_message>
<xml_diff>
--- a/sql/library-abq-all.xlsx
+++ b/sql/library-abq-all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kbowman5\little-library\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93581B98-C45A-4122-87D5-3BEB52B2CBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07652D76-E2DD-467E-BD25-6AF0EEB1CE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6435" yWindow="1470" windowWidth="29775" windowHeight="19245" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
+    <workbookView xWindow="23595" yWindow="7935" windowWidth="29775" windowHeight="19245" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
   </bookViews>
   <sheets>
     <sheet name="library-abq-all" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="184">
   <si>
     <t>La Luz</t>
   </si>
@@ -585,6 +585,12 @@
   </si>
   <si>
     <t>Young Adult</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -648,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -663,6 +669,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -981,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF696C8F-C0BA-4CFB-9733-D4AF25C2BA9E}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -991,7 +1003,7 @@
     <col min="2" max="2" width="15.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="46.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -1013,7 +1025,7 @@
       <c r="D1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>152</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1039,8 +1051,8 @@
       <c r="D2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="2" t="b">
-        <v>1</v>
+      <c r="E2" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F2" s="2">
         <v>35.181539999999998</v>
@@ -1062,8 +1074,8 @@
       <c r="D3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="2" t="b">
-        <v>0</v>
+      <c r="E3" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F3" s="2">
         <v>35.188479999999998</v>
@@ -1088,8 +1100,8 @@
       <c r="D4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="2" t="b">
-        <v>1</v>
+      <c r="E4" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F4" s="2">
         <v>35.153370000000002</v>
@@ -1114,8 +1126,8 @@
       <c r="D5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="2" t="b">
-        <v>0</v>
+      <c r="E5" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F5" s="2">
         <v>35.131599999999999</v>
@@ -1140,8 +1152,8 @@
       <c r="D6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="2" t="b">
-        <v>1</v>
+      <c r="E6" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F6" s="2">
         <v>35.123800000000003</v>
@@ -1166,8 +1178,8 @@
       <c r="D7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="2" t="b">
-        <v>0</v>
+      <c r="E7" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F7" s="2">
         <v>35.121979099999997</v>
@@ -1192,8 +1204,8 @@
       <c r="D8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="2" t="b">
-        <v>1</v>
+      <c r="E8" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F8" s="2">
         <v>35.117571099999999</v>
@@ -1218,8 +1230,8 @@
       <c r="D9" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="2" t="b">
-        <v>0</v>
+      <c r="E9" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F9" s="2">
         <v>35.128052199999999</v>
@@ -1241,8 +1253,8 @@
       <c r="C10" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="2" t="b">
-        <v>1</v>
+      <c r="E10" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F10" s="2">
         <v>35.119197300000003</v>
@@ -1267,8 +1279,8 @@
       <c r="D11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="2" t="b">
-        <v>0</v>
+      <c r="E11" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F11" s="2">
         <v>35.0847689</v>
@@ -1290,8 +1302,8 @@
       <c r="C12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="2" t="b">
-        <v>1</v>
+      <c r="E12" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F12" s="2">
         <v>35.069223299999997</v>
@@ -1313,8 +1325,8 @@
       <c r="C13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="2" t="b">
-        <v>0</v>
+      <c r="E13" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F13" s="2">
         <v>35.072239699999997</v>
@@ -1339,8 +1351,8 @@
       <c r="D14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="2" t="b">
-        <v>1</v>
+      <c r="E14" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F14" s="2">
         <v>35.0599913</v>
@@ -1362,8 +1374,8 @@
       <c r="C15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="2" t="b">
-        <v>0</v>
+      <c r="E15" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F15" s="2">
         <v>35.0658277</v>
@@ -1388,8 +1400,8 @@
       <c r="D16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="2" t="b">
-        <v>1</v>
+      <c r="E16" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F16" s="2">
         <v>35.066689099999998</v>
@@ -1411,8 +1423,8 @@
       <c r="D17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="2" t="b">
-        <v>0</v>
+      <c r="E17" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F17" s="2">
         <v>35.071187799999997</v>
@@ -1431,8 +1443,8 @@
       <c r="C18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="2" t="b">
-        <v>1</v>
+      <c r="E18" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F18" s="2">
         <v>35.074612399999999</v>
@@ -1457,8 +1469,8 @@
       <c r="D19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="2" t="b">
-        <v>0</v>
+      <c r="E19" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F19" s="2">
         <v>35.070069500000002</v>
@@ -1483,8 +1495,8 @@
       <c r="D20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="2" t="b">
-        <v>1</v>
+      <c r="E20" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F20" s="2">
         <v>35.206665899999997</v>
@@ -1509,8 +1521,8 @@
       <c r="D21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="2" t="b">
-        <v>1</v>
+      <c r="E21" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F21" s="2">
         <v>35.208756600000001</v>
@@ -1535,8 +1547,8 @@
       <c r="D22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="2" t="b">
-        <v>1</v>
+      <c r="E22" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F22" s="2">
         <v>35.214978299999999</v>
@@ -1558,8 +1570,8 @@
       <c r="D23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="2" t="b">
-        <v>1</v>
+      <c r="E23" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F23" s="2">
         <v>35.223036100000002</v>
@@ -1584,8 +1596,8 @@
       <c r="D24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="2" t="b">
-        <v>1</v>
+      <c r="E24" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F24" s="2">
         <v>35.192672199999997</v>
@@ -1610,8 +1622,8 @@
       <c r="D25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="2" t="b">
-        <v>1</v>
+      <c r="E25" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F25" s="2">
         <v>35.211012799999999</v>
@@ -1636,8 +1648,8 @@
       <c r="D26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="2" t="b">
-        <v>1</v>
+      <c r="E26" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F26" s="2">
         <v>35.1563126</v>
@@ -1662,8 +1674,8 @@
       <c r="D27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="2" t="b">
-        <v>1</v>
+      <c r="E27" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F27" s="2">
         <v>35.244074900000001</v>
@@ -1688,8 +1700,8 @@
       <c r="D28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="2" t="b">
-        <v>1</v>
+      <c r="E28" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F28" s="2">
         <v>35.137509700000003</v>
@@ -1711,8 +1723,8 @@
       <c r="D29" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E29" s="2" t="b">
-        <v>1</v>
+      <c r="E29" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F29" s="2">
         <v>35.157112499999997</v>
@@ -1735,8 +1747,8 @@
       <c r="D30" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E30" s="2" t="b">
-        <v>0</v>
+      <c r="E30" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F30" s="2">
         <v>35.155270299999998</v>
@@ -1758,8 +1770,8 @@
       <c r="D31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="2" t="b">
-        <v>1</v>
+      <c r="E31" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="F31" s="2">
         <v>35.165264899999997</v>
@@ -1778,7 +1790,7 @@
       <c r="C32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E32" s="2" t="b">
+      <c r="E32" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F32" s="2">
@@ -1801,8 +1813,8 @@
       <c r="D33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E33" s="2" t="b">
-        <v>0</v>
+      <c r="E33" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F33" s="2">
         <v>35.126519899999998</v>
@@ -1824,8 +1836,8 @@
       <c r="D34" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E34" s="2" t="b">
-        <v>0</v>
+      <c r="E34" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F34" s="4">
         <v>35.071759999999998</v>
@@ -1850,7 +1862,7 @@
       <c r="D35" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E35" s="2" t="b">
+      <c r="E35" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F35" s="4">
@@ -1876,8 +1888,8 @@
       <c r="D36" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="2" t="b">
-        <v>0</v>
+      <c r="E36" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F36" s="4">
         <v>35.159329999999997</v>
@@ -1902,8 +1914,8 @@
       <c r="D37" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E37" s="2" t="b">
-        <v>0</v>
+      <c r="E37" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F37" s="4">
         <v>35.079929999999997</v>
@@ -1928,8 +1940,8 @@
       <c r="D38" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E38" s="2" t="b">
-        <v>0</v>
+      <c r="E38" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F38" s="4">
         <v>35.124859999999998</v>
@@ -1954,8 +1966,8 @@
       <c r="D39" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E39" s="2" t="b">
-        <v>0</v>
+      <c r="E39" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F39" s="4">
         <v>35.070410000000003</v>
@@ -1980,8 +1992,8 @@
       <c r="D40" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E40" s="2" t="b">
-        <v>0</v>
+      <c r="E40" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F40" s="4">
         <v>35.075949999999999</v>
@@ -2006,8 +2018,8 @@
       <c r="D41" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E41" s="2" t="b">
-        <v>0</v>
+      <c r="E41" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F41" s="4">
         <v>35.120849999999997</v>
@@ -2032,8 +2044,8 @@
       <c r="D42" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E42" s="2" t="b">
-        <v>0</v>
+      <c r="E42" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F42" s="4">
         <v>35.086069999999999</v>
@@ -2058,8 +2070,8 @@
       <c r="D43" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E43" s="2" t="b">
-        <v>0</v>
+      <c r="E43" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F43" s="4">
         <v>35.132750000000001</v>
@@ -2084,8 +2096,8 @@
       <c r="D44" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E44" s="2" t="b">
-        <v>0</v>
+      <c r="E44" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F44" s="4">
         <v>35.086210000000001</v>
@@ -2110,8 +2122,8 @@
       <c r="D45" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E45" s="2" t="b">
-        <v>0</v>
+      <c r="E45" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F45" s="4">
         <v>35.167819999999999</v>
@@ -2136,8 +2148,8 @@
       <c r="D46" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E46" s="2" t="b">
-        <v>0</v>
+      <c r="E46" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F46" s="4">
         <v>35.069020000000002</v>
@@ -2162,8 +2174,8 @@
       <c r="D47" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E47" s="2" t="b">
-        <v>0</v>
+      <c r="E47" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F47" s="4">
         <v>35.073140000000002</v>
@@ -2188,8 +2200,8 @@
       <c r="D48" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E48" s="2" t="b">
-        <v>0</v>
+      <c r="E48" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F48" s="4">
         <v>35.018900000000002</v>
@@ -2214,8 +2226,8 @@
       <c r="D49" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E49" s="2" t="b">
-        <v>0</v>
+      <c r="E49" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F49" s="4">
         <v>35.084029999999998</v>
@@ -2240,8 +2252,8 @@
       <c r="D50" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E50" s="2" t="b">
-        <v>0</v>
+      <c r="E50" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F50" s="4">
         <v>35.149520000000003</v>
@@ -2266,8 +2278,8 @@
       <c r="D51" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E51" s="2" t="b">
-        <v>0</v>
+      <c r="E51" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F51" s="4">
         <v>35.108040000000003</v>
@@ -2292,8 +2304,8 @@
       <c r="D52" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E52" s="2" t="b">
-        <v>0</v>
+      <c r="E52" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="F52" s="4">
         <v>35.051650000000002</v>
@@ -2313,5 +2325,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
noticed bug with previously add profile blocks
</commit_message>
<xml_diff>
--- a/sql/library-abq-all.xlsx
+++ b/sql/library-abq-all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kbowman5\little-library\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2E1F8F-6416-4B33-88F5-BBF7C57774A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A192DE30-875A-4CA0-B671-CC7597D54AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21630" yWindow="6135" windowWidth="35625" windowHeight="19245" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
+    <workbookView xWindow="-35685" yWindow="2970" windowWidth="35625" windowHeight="19035" xr2:uid="{4EF4C7CD-7A5B-42CB-8670-A2ACA8F0D658}"/>
   </bookViews>
   <sheets>
     <sheet name="library-abq-all" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="183">
   <si>
     <t>La Luz</t>
   </si>
@@ -585,6 +585,9 @@
   </si>
   <si>
     <t>Official</t>
+  </si>
+  <si>
+    <t>library_image_url</t>
   </si>
 </sst>
 </file>
@@ -979,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF696C8F-C0BA-4CFB-9733-D4AF25C2BA9E}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -992,15 +995,16 @@
     <col min="3" max="3" width="28.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="46.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="26.85546875" style="2"/>
+    <col min="6" max="6" width="16" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="26.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -1017,22 +1021,25 @@
         <v>130</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>64</v>
       </c>
@@ -1042,20 +1049,20 @@
       <c r="E2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>35.181539999999998</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>-106.4979</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K2" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
         <v>61</v>
       </c>
@@ -1065,23 +1072,23 @@
       <c r="E3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>35.188479999999998</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>-106.55759</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K3" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>159</v>
       </c>
@@ -1091,23 +1098,23 @@
       <c r="E4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>35.153370000000002</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>-106.53207999999999</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="K4" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>160</v>
       </c>
@@ -1117,23 +1124,23 @@
       <c r="E5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>35.131599999999999</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>-106.49453</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="K5" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="89.25" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>161</v>
       </c>
@@ -1143,23 +1150,23 @@
       <c r="E6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>35.123800000000003</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>-106.52722</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="K6" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>162</v>
       </c>
@@ -1169,23 +1176,23 @@
       <c r="E7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>35.121979099999997</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>-106.5167993</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="K7" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>50</v>
       </c>
@@ -1195,23 +1202,23 @@
       <c r="E8" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>35.117571099999999</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>-106.582446</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="K8" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="127.5" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>47</v>
       </c>
@@ -1221,46 +1228,46 @@
       <c r="E9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>35.128052199999999</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>-106.5694163</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K9" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>163</v>
       </c>
       <c r="E10" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>35.119197300000003</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>-106.55185299999999</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="K10" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>164</v>
       </c>
@@ -1270,69 +1277,69 @@
       <c r="E11" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>35.0847689</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>-106.5585485</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K11" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>165</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>35.069223299999997</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>-106.4901282</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K12" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>166</v>
       </c>
       <c r="E13" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>35.072239699999997</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>-106.58912599999999</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K13" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>167</v>
       </c>
@@ -1342,46 +1349,46 @@
       <c r="E14" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>35.0599913</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>-106.5931535</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K14" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>35.0658277</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>-106.6031375</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+      <c r="K15" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="102" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>36</v>
       </c>
@@ -1391,20 +1398,20 @@
       <c r="E16" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>35.066689099999998</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>-106.60363719999999</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10" ht="102" x14ac:dyDescent="0.25">
+      <c r="K16" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" ht="102" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>168</v>
       </c>
@@ -1414,43 +1421,43 @@
       <c r="E17" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>35.071187799999997</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>-106.59730279999999</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K17" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>169</v>
       </c>
       <c r="E18" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>35.074612399999999</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>-106.6014539</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="3:10" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="K18" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" ht="127.5" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>30</v>
       </c>
@@ -1460,23 +1467,23 @@
       <c r="E19" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>35.070069500000002</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>-106.573905</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K19" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
         <v>170</v>
       </c>
@@ -1486,23 +1493,23 @@
       <c r="E20" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>35.206665899999997</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>-106.6733902</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="3:10" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="K20" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" ht="76.5" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1512,23 +1519,23 @@
       <c r="E21" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>35.208756600000001</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>-106.67306859999999</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="3:10" ht="102" x14ac:dyDescent="0.25">
+      <c r="K21" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" ht="102" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>171</v>
       </c>
@@ -1538,20 +1545,20 @@
       <c r="E22" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>35.214978299999999</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>-106.66908359999999</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="K22" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>172</v>
       </c>
@@ -1561,23 +1568,23 @@
       <c r="E23" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>35.223036100000002</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>-106.6857408</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="K23" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" ht="114.75" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>173</v>
       </c>
@@ -1587,23 +1594,23 @@
       <c r="E24" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>35.192672199999997</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>-106.6716868</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K24" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
         <v>174</v>
       </c>
@@ -1613,23 +1620,23 @@
       <c r="E25" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F25" s="2">
+      <c r="G25" s="2">
         <v>35.211012799999999</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>-106.72355640000001</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="3:10" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="K25" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" ht="76.5" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>175</v>
       </c>
@@ -1639,23 +1646,23 @@
       <c r="E26" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>35.1563126</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>-106.6916086</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K26" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
         <v>176</v>
       </c>
@@ -1665,23 +1672,23 @@
       <c r="E27" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F27" s="2">
+      <c r="G27" s="2">
         <v>35.244074900000001</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>-106.6640871</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="3:10" ht="102" x14ac:dyDescent="0.25">
+      <c r="K27" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" ht="102" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
         <v>10</v>
       </c>
@@ -1691,20 +1698,20 @@
       <c r="E28" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F28" s="2">
+      <c r="G28" s="2">
         <v>35.137509700000003</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>-106.70054519999999</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="3:10" ht="51" x14ac:dyDescent="0.25">
+      <c r="K28" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" ht="51" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>177</v>
       </c>
@@ -1714,21 +1721,21 @@
       <c r="E29" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
         <v>35.157112499999997</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>-106.717429</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="J29" s="5"/>
+      <c r="K29" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1738,20 +1745,20 @@
       <c r="E30" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F30" s="2">
+      <c r="G30" s="2">
         <v>35.155270299999998</v>
       </c>
-      <c r="G30" s="2">
+      <c r="H30" s="2">
         <v>-106.7097816</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="I30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K30" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
         <v>178</v>
       </c>
@@ -1761,40 +1768,40 @@
       <c r="E31" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F31" s="2">
+      <c r="G31" s="2">
         <v>35.165264899999997</v>
       </c>
-      <c r="G31" s="2">
+      <c r="H31" s="2">
         <v>-106.6778819</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J31" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K31" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
         <v>179</v>
       </c>
       <c r="E32" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F32" s="2">
+      <c r="G32" s="2">
         <v>35.170054899999997</v>
       </c>
-      <c r="G32" s="2">
+      <c r="H32" s="2">
         <v>-106.67219350000001</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="K32" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
         <v>180</v>
       </c>
@@ -1804,20 +1811,20 @@
       <c r="E33" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F33" s="2">
+      <c r="G33" s="2">
         <v>35.126519899999998</v>
       </c>
-      <c r="G33" s="2">
+      <c r="H33" s="2">
         <v>-106.6521122</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="I33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C34" s="4" t="s">
         <v>74</v>
       </c>
@@ -1827,23 +1834,23 @@
       <c r="E34" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F34" s="4">
+      <c r="G34" s="4">
         <v>35.071759999999998</v>
       </c>
-      <c r="G34" s="4">
+      <c r="H34" s="4">
         <v>-106.70972</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="I34" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C35" s="4" t="s">
         <v>75</v>
       </c>
@@ -1853,23 +1860,23 @@
       <c r="E35" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F35" s="4">
+      <c r="G35" s="4">
         <v>35.0779</v>
       </c>
-      <c r="G35" s="4">
+      <c r="H35" s="4">
         <v>-106.72486000000001</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="I35" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="J35" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="K35" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="3:10" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C36" s="4" t="s">
         <v>76</v>
       </c>
@@ -1879,23 +1886,23 @@
       <c r="E36" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F36" s="4">
+      <c r="G36" s="4">
         <v>35.159329999999997</v>
       </c>
-      <c r="G36" s="4">
+      <c r="H36" s="4">
         <v>-106.5558</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="J36" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="K36" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C37" s="4" t="s">
         <v>77</v>
       </c>
@@ -1905,23 +1912,23 @@
       <c r="E37" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F37" s="4">
+      <c r="G37" s="4">
         <v>35.079929999999997</v>
       </c>
-      <c r="G37" s="4">
+      <c r="H37" s="4">
         <v>-106.38930000000001</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="I37" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="J37" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="K37" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C38" s="4" t="s">
         <v>78</v>
       </c>
@@ -1931,23 +1938,23 @@
       <c r="E38" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F38" s="4">
+      <c r="G38" s="4">
         <v>35.124859999999998</v>
       </c>
-      <c r="G38" s="4">
+      <c r="H38" s="4">
         <v>-106.58564</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="I38" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="J38" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="K38" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="3:10" ht="102" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:11" ht="102" x14ac:dyDescent="0.2">
       <c r="C39" s="4" t="s">
         <v>79</v>
       </c>
@@ -1957,23 +1964,23 @@
       <c r="E39" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F39" s="4">
+      <c r="G39" s="4">
         <v>35.070410000000003</v>
       </c>
-      <c r="G39" s="4">
+      <c r="H39" s="4">
         <v>-106.61281</v>
       </c>
-      <c r="H39" s="4" t="s">
+      <c r="I39" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="J39" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C40" s="4" t="s">
         <v>80</v>
       </c>
@@ -1983,23 +1990,23 @@
       <c r="E40" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F40" s="4">
+      <c r="G40" s="4">
         <v>35.075949999999999</v>
       </c>
-      <c r="G40" s="4">
+      <c r="H40" s="4">
         <v>-106.56204</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="I40" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="J40" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="K40" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C41" s="4" t="s">
         <v>81</v>
       </c>
@@ -2009,23 +2016,23 @@
       <c r="E41" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F41" s="4">
+      <c r="G41" s="4">
         <v>35.120849999999997</v>
       </c>
-      <c r="G41" s="4">
+      <c r="H41" s="4">
         <v>-106.51611</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="I41" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="J41" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="K41" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C42" s="4" t="s">
         <v>82</v>
       </c>
@@ -2035,23 +2042,23 @@
       <c r="E42" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F42" s="4">
+      <c r="G42" s="4">
         <v>35.086069999999999</v>
       </c>
-      <c r="G42" s="4">
+      <c r="H42" s="4">
         <v>-106.49758</v>
       </c>
-      <c r="H42" s="4" t="s">
+      <c r="I42" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="J42" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="K42" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C43" s="4" t="s">
         <v>83</v>
       </c>
@@ -2061,23 +2068,23 @@
       <c r="E43" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F43" s="4">
+      <c r="G43" s="4">
         <v>35.132750000000001</v>
       </c>
-      <c r="G43" s="4">
+      <c r="H43" s="4">
         <v>-106.64831</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="I43" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="J43" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="K43" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C44" s="4" t="s">
         <v>84</v>
       </c>
@@ -2087,23 +2094,23 @@
       <c r="E44" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F44" s="4">
+      <c r="G44" s="4">
         <v>35.086210000000001</v>
       </c>
-      <c r="G44" s="4">
+      <c r="H44" s="4">
         <v>-106.65331999999999</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="I44" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="J44" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="K44" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="3:10" ht="102" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:11" ht="102" x14ac:dyDescent="0.2">
       <c r="C45" s="4" t="s">
         <v>85</v>
       </c>
@@ -2113,23 +2120,23 @@
       <c r="E45" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F45" s="4">
+      <c r="G45" s="4">
         <v>35.167819999999999</v>
       </c>
-      <c r="G45" s="4">
+      <c r="H45" s="4">
         <v>-106.62716</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="I45" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="J45" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="K45" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C46" s="4" t="s">
         <v>86</v>
       </c>
@@ -2139,23 +2146,23 @@
       <c r="E46" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F46" s="4">
+      <c r="G46" s="4">
         <v>35.069020000000002</v>
       </c>
-      <c r="G46" s="4">
+      <c r="H46" s="4">
         <v>-106.57723</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="I46" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="J46" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J46" s="2" t="s">
+      <c r="K46" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C47" s="4" t="s">
         <v>87</v>
       </c>
@@ -2165,23 +2172,23 @@
       <c r="E47" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F47" s="4">
+      <c r="G47" s="4">
         <v>35.073140000000002</v>
       </c>
-      <c r="G47" s="4">
+      <c r="H47" s="4">
         <v>-106.64546</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="I47" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="J47" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="K47" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C48" s="4" t="s">
         <v>88</v>
       </c>
@@ -2191,23 +2198,23 @@
       <c r="E48" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F48" s="4">
+      <c r="G48" s="4">
         <v>35.018900000000002</v>
       </c>
-      <c r="G48" s="4">
+      <c r="H48" s="4">
         <v>-106.68216</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="I48" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="J48" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="K48" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="3:10" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:11" ht="89.25" x14ac:dyDescent="0.2">
       <c r="C49" s="4" t="s">
         <v>89</v>
       </c>
@@ -2217,23 +2224,23 @@
       <c r="E49" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F49" s="4">
+      <c r="G49" s="4">
         <v>35.084029999999998</v>
       </c>
-      <c r="G49" s="4">
+      <c r="H49" s="4">
         <v>-106.64216999999999</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="I49" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="J49" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J49" s="2" t="s">
+      <c r="K49" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="3:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C50" s="4" t="s">
         <v>90</v>
       </c>
@@ -2243,23 +2250,23 @@
       <c r="E50" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F50" s="4">
+      <c r="G50" s="4">
         <v>35.149520000000003</v>
       </c>
-      <c r="G50" s="4">
+      <c r="H50" s="4">
         <v>-106.71614</v>
       </c>
-      <c r="H50" s="4" t="s">
+      <c r="I50" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="J50" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J50" s="2" t="s">
+      <c r="K50" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="3:10" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="C51" s="4" t="s">
         <v>91</v>
       </c>
@@ -2269,23 +2276,23 @@
       <c r="E51" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F51" s="4">
+      <c r="G51" s="4">
         <v>35.108040000000003</v>
       </c>
-      <c r="G51" s="4">
+      <c r="H51" s="4">
         <v>-106.55294000000001</v>
       </c>
-      <c r="H51" s="4" t="s">
+      <c r="I51" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I51" s="2" t="s">
+      <c r="J51" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J51" s="2" t="s">
+      <c r="K51" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="3:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C52" s="4" t="s">
         <v>92</v>
       </c>
@@ -2295,19 +2302,19 @@
       <c r="E52" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F52" s="4">
+      <c r="G52" s="4">
         <v>35.051650000000002</v>
       </c>
-      <c r="G52" s="4">
+      <c r="H52" s="4">
         <v>-106.75161</v>
       </c>
-      <c r="H52" s="4" t="s">
+      <c r="I52" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="I52" s="2" t="s">
+      <c r="J52" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J52" s="2" t="s">
+      <c r="K52" s="2" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>